<commit_message>
made my own daily sched table using row & colspan
</commit_message>
<xml_diff>
--- a/Daily Schedule - Detailed Study Guide Plan - Week 1.xlsx
+++ b/Daily Schedule - Detailed Study Guide Plan - Week 1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/54037f66d77c46de/Desktop/Full-Stack Developer Study Plan/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/54037f66d77c46de/Desktop/Full-Stack Developer Study Plan/Week 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="55" documentId="8_{37F14603-7835-45D1-9366-2EF83A7B62AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9AE0D6C2-8BCF-4154-B584-111D7F01C3EB}"/>
+  <xr:revisionPtr revIDLastSave="70" documentId="8_{37F14603-7835-45D1-9366-2EF83A7B62AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E5F4777-E84D-4614-BFCD-779A0F5FA339}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{131ED3EB-DB14-4793-ADA5-E51D81EA1C6E}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="84">
   <si>
     <t>Day 1 - Introduction to HTML - 02/27/2025</t>
   </si>
@@ -286,18 +286,6 @@
   </si>
   <si>
     <t>Share my first website online</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=BczLWImAmBk</t>
-  </si>
-  <si>
-    <t>Forms</t>
-  </si>
-  <si>
-    <t>rowspan &amp; colspan</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=iuSKGuWWNGA</t>
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=FHb9JobDs2o</t>
@@ -481,7 +469,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -497,15 +485,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -525,9 +504,19 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -547,6 +536,139 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>563880</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle: Rounded Corners 1">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86F025BA-E5AE-4877-D179-A4E819CA0044}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1645920" y="3063240"/>
+          <a:ext cx="1684020" cy="777240"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-PH" sz="1100"/>
+            <a:t>FORMS</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>632460</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle: Rounded Corners 2">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1EFDB58D-1E40-4CC1-AF27-433ED075D630}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3672840" y="3063240"/>
+          <a:ext cx="1684020" cy="777240"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-PH" sz="1100"/>
+            <a:t>ROWSPAN &amp; COLSPAN</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -940,31 +1062,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
     </row>
     <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="13" t="s">
+      <c r="B2" s="9"/>
+      <c r="C2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="13" t="s">
+      <c r="D2" s="11"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="11"/>
       <c r="H2" s="2" t="s">
         <v>4</v>
       </c>
@@ -976,15 +1098,15 @@
       <c r="B3" s="3">
         <v>6.25E-2</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="9" t="s">
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="9"/>
+      <c r="G3" s="15"/>
       <c r="H3" s="4" t="s">
         <v>7</v>
       </c>
@@ -996,15 +1118,15 @@
       <c r="B4" s="3">
         <v>0.10416666666666667</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="10" t="s">
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="9"/>
+      <c r="G4" s="15"/>
       <c r="H4" s="4" t="s">
         <v>7</v>
       </c>
@@ -1016,15 +1138,15 @@
       <c r="B5" s="3">
         <v>0.14583333333333334</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="9" t="s">
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="9"/>
+      <c r="G5" s="15"/>
       <c r="H5" s="4" t="s">
         <v>7</v>
       </c>
@@ -1036,15 +1158,15 @@
       <c r="B6" s="3">
         <v>0.16666666666666666</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="9" t="s">
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="9"/>
+      <c r="G6" s="15"/>
       <c r="H6" s="4" t="s">
         <v>7</v>
       </c>
@@ -1056,15 +1178,15 @@
       <c r="B7" s="3">
         <v>0.20833333333333334</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="9" t="s">
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="9"/>
+      <c r="G7" s="15"/>
       <c r="H7" s="4" t="s">
         <v>7</v>
       </c>
@@ -1076,26 +1198,21 @@
       <c r="B8" s="3">
         <v>0.25</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="9" t="s">
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="9"/>
+      <c r="G8" s="15"/>
       <c r="H8" s="4" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="C3:E3"/>
     <mergeCell ref="C5:E5"/>
     <mergeCell ref="C6:E6"/>
     <mergeCell ref="C7:E7"/>
@@ -1107,6 +1224,11 @@
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="C4:E4"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="C3:E3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F4" r:id="rId1" xr:uid="{0649C151-4FF5-41ED-8C94-466E40481E6E}"/>
@@ -1120,7 +1242,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="F7" activeCellId="2" sqref="G13 F4:G4 F7:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1138,31 +1260,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
     </row>
     <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="13" t="s">
+      <c r="B2" s="9"/>
+      <c r="C2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="13" t="s">
+      <c r="D2" s="11"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="11"/>
       <c r="H2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1174,24 +1296,20 @@
       <c r="B3" s="3">
         <v>6.25E-2</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="9" t="s">
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="9"/>
+      <c r="G3" s="15"/>
       <c r="H3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>84</v>
-      </c>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
     </row>
     <row r="4" spans="1:10" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
@@ -1200,24 +1318,20 @@
       <c r="B4" s="3">
         <v>0.10416666666666667</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
       <c r="F4" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="9"/>
+      <c r="G4" s="15"/>
       <c r="H4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>85</v>
-      </c>
+      <c r="I4" s="18"/>
+      <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
@@ -1226,15 +1340,15 @@
       <c r="B5" s="3">
         <v>0.14583333333333334</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="9" t="s">
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="9"/>
+      <c r="G5" s="15"/>
       <c r="H5" s="4" t="s">
         <v>7</v>
       </c>
@@ -1246,15 +1360,15 @@
       <c r="B6" s="3">
         <v>0.16666666666666666</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="9" t="s">
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="9"/>
+      <c r="G6" s="15"/>
       <c r="H6" s="4" t="s">
         <v>7</v>
       </c>
@@ -1266,17 +1380,17 @@
       <c r="B7" s="3">
         <v>0.20833333333333334</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
       <c r="F7" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="G7" s="9"/>
+        <v>82</v>
+      </c>
+      <c r="G7" s="15"/>
       <c r="H7" s="7" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1286,27 +1400,21 @@
       <c r="B8" s="3">
         <v>0.25</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="9" t="s">
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="9"/>
+      <c r="G8" s="15"/>
       <c r="H8" s="4" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="F3:G3"/>
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="C8:E8"/>
@@ -1317,14 +1425,19 @@
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="C6:E6"/>
     <mergeCell ref="F6:G6"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="F3:G3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F4" r:id="rId1" xr:uid="{CA69D407-ADBF-4FF3-B1FE-5BA0923AB350}"/>
-    <hyperlink ref="I4" r:id="rId2" xr:uid="{00E3C4FA-7F90-4263-B91E-1FA07B7A07A0}"/>
-    <hyperlink ref="J4" r:id="rId3" xr:uid="{25F5EBCC-8FBC-4D20-83B9-0869803AA8CE}"/>
-    <hyperlink ref="F7" r:id="rId4" xr:uid="{403CB1B1-D116-4F75-9F15-EA732E8F9EA4}"/>
+    <hyperlink ref="F7" r:id="rId2" xr:uid="{403CB1B1-D116-4F75-9F15-EA732E8F9EA4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1348,31 +1461,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
     </row>
     <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="13" t="s">
+      <c r="B2" s="9"/>
+      <c r="C2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="13" t="s">
+      <c r="D2" s="11"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="11"/>
       <c r="H2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1384,15 +1497,15 @@
       <c r="B3" s="3">
         <v>6.25E-2</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="9" t="s">
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="9"/>
+      <c r="G3" s="15"/>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1402,15 +1515,15 @@
       <c r="B4" s="3">
         <v>0.10416666666666667</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
       <c r="F4" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="9"/>
+      <c r="G4" s="15"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1420,15 +1533,15 @@
       <c r="B5" s="3">
         <v>0.14583333333333334</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="9" t="s">
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="9"/>
+      <c r="G5" s="15"/>
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -1438,15 +1551,15 @@
       <c r="B6" s="3">
         <v>0.16666666666666666</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="9" t="s">
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="9"/>
+      <c r="G6" s="15"/>
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -1456,15 +1569,15 @@
       <c r="B7" s="3">
         <v>0.20833333333333334</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="9" t="s">
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="G7" s="9"/>
+      <c r="G7" s="15"/>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1474,25 +1587,19 @@
       <c r="B8" s="3">
         <v>0.25</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="9" t="s">
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="G8" s="9"/>
+      <c r="G8" s="15"/>
       <c r="H8" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="F3:G3"/>
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="C8:E8"/>
@@ -1503,6 +1610,12 @@
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="C6:E6"/>
     <mergeCell ref="F6:G6"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="F3:G3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F4" r:id="rId1" xr:uid="{4257805A-436E-4161-B8F5-14DBE7520749}"/>
@@ -1532,31 +1645,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
     </row>
     <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="13" t="s">
+      <c r="B2" s="9"/>
+      <c r="C2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="13" t="s">
+      <c r="D2" s="11"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="11"/>
       <c r="H2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1568,15 +1681,15 @@
       <c r="B3" s="3">
         <v>6.25E-2</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="9" t="s">
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="G3" s="9"/>
+      <c r="G3" s="15"/>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1586,15 +1699,15 @@
       <c r="B4" s="3">
         <v>0.10416666666666667</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
       <c r="F4" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="G4" s="9"/>
+      <c r="G4" s="15"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1604,15 +1717,15 @@
       <c r="B5" s="3">
         <v>0.14583333333333334</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="9" t="s">
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="G5" s="9"/>
+      <c r="G5" s="15"/>
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -1622,15 +1735,15 @@
       <c r="B6" s="3">
         <v>0.16666666666666666</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="9" t="s">
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="9"/>
+      <c r="G6" s="15"/>
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -1640,15 +1753,15 @@
       <c r="B7" s="3">
         <v>0.20833333333333334</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
       <c r="F7" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="G7" s="9"/>
+      <c r="G7" s="15"/>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1658,25 +1771,19 @@
       <c r="B8" s="3">
         <v>0.25</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="9" t="s">
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="G8" s="9"/>
+      <c r="G8" s="15"/>
       <c r="H8" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="F3:G3"/>
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="C8:E8"/>
@@ -1687,6 +1794,12 @@
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="C6:E6"/>
     <mergeCell ref="F6:G6"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="F3:G3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F4" r:id="rId1" xr:uid="{DC0E6990-69A5-43AE-B703-81524696C1B6}"/>
@@ -1717,31 +1830,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
     </row>
     <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="13" t="s">
+      <c r="B2" s="9"/>
+      <c r="C2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="13" t="s">
+      <c r="D2" s="11"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="11"/>
       <c r="H2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1753,15 +1866,15 @@
       <c r="B3" s="3">
         <v>6.25E-2</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="9" t="s">
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="9"/>
+      <c r="G3" s="15"/>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1771,15 +1884,15 @@
       <c r="B4" s="3">
         <v>0.10416666666666667</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
       <c r="F4" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="G4" s="9"/>
+      <c r="G4" s="15"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1789,15 +1902,15 @@
       <c r="B5" s="3">
         <v>0.14583333333333334</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="9" t="s">
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="9"/>
+      <c r="G5" s="15"/>
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -1807,15 +1920,15 @@
       <c r="B6" s="3">
         <v>0.16666666666666666</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="9" t="s">
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="9"/>
+      <c r="G6" s="15"/>
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1825,15 +1938,15 @@
       <c r="B7" s="3">
         <v>0.20833333333333334</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="9" t="s">
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="G7" s="9"/>
+      <c r="G7" s="15"/>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1843,25 +1956,19 @@
       <c r="B8" s="3">
         <v>0.25</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="9" t="s">
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="G8" s="9"/>
+      <c r="G8" s="15"/>
       <c r="H8" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="F3:G3"/>
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="C8:E8"/>
@@ -1872,6 +1979,12 @@
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="C6:E6"/>
     <mergeCell ref="F6:G6"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="F3:G3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F4" r:id="rId1" xr:uid="{7363BFB9-59B9-41E4-94A2-43DBF92C838E}"/>
@@ -1901,31 +2014,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
     </row>
     <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="13" t="s">
+      <c r="B2" s="9"/>
+      <c r="C2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="13" t="s">
+      <c r="D2" s="11"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="11"/>
       <c r="H2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1937,15 +2050,15 @@
       <c r="B3" s="3">
         <v>6.25E-2</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="9" t="s">
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="G3" s="9"/>
+      <c r="G3" s="15"/>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1955,15 +2068,15 @@
       <c r="B4" s="3">
         <v>0.10416666666666667</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
       <c r="F4" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="G4" s="9"/>
+      <c r="G4" s="15"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1973,15 +2086,15 @@
       <c r="B5" s="3">
         <v>0.14583333333333334</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="9" t="s">
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="G5" s="9"/>
+      <c r="G5" s="15"/>
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -1991,15 +2104,15 @@
       <c r="B6" s="3">
         <v>0.16666666666666666</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="9" t="s">
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="9"/>
+      <c r="G6" s="15"/>
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2009,15 +2122,15 @@
       <c r="B7" s="3">
         <v>0.20833333333333334</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="9" t="s">
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="G7" s="9"/>
+      <c r="G7" s="15"/>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2027,25 +2140,19 @@
       <c r="B8" s="3">
         <v>0.25</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="9" t="s">
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="G8" s="9"/>
+      <c r="G8" s="15"/>
       <c r="H8" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="F3:G3"/>
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="C8:E8"/>
@@ -2056,6 +2163,12 @@
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="C6:E6"/>
     <mergeCell ref="F6:G6"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="F3:G3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F4" r:id="rId1" xr:uid="{FC9BA8A3-E4A7-4AA4-A429-F1F08DE2C02D}"/>
@@ -2085,31 +2198,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
     </row>
     <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="13" t="s">
+      <c r="B2" s="9"/>
+      <c r="C2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="13" t="s">
+      <c r="D2" s="11"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="11"/>
       <c r="H2" s="2" t="s">
         <v>4</v>
       </c>
@@ -2121,15 +2234,15 @@
       <c r="B3" s="3">
         <v>6.25E-2</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="9" t="s">
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="G3" s="9"/>
+      <c r="G3" s="15"/>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2139,15 +2252,15 @@
       <c r="B4" s="3">
         <v>0.10416666666666667</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="9" t="s">
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="G4" s="9"/>
+      <c r="G4" s="15"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2157,15 +2270,15 @@
       <c r="B5" s="3">
         <v>0.14583333333333334</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="9" t="s">
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="G5" s="9"/>
+      <c r="G5" s="15"/>
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -2175,15 +2288,15 @@
       <c r="B6" s="3">
         <v>0.16666666666666666</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="9" t="s">
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="9"/>
+      <c r="G6" s="15"/>
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -2193,15 +2306,15 @@
       <c r="B7" s="3">
         <v>0.20833333333333334</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="9" t="s">
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="G7" s="9"/>
+      <c r="G7" s="15"/>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -2211,25 +2324,19 @@
       <c r="B8" s="3">
         <v>0.25</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="9" t="s">
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="G8" s="9"/>
+      <c r="G8" s="15"/>
       <c r="H8" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="F3:G3"/>
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="C8:E8"/>
@@ -2240,6 +2347,12 @@
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="C6:E6"/>
     <mergeCell ref="F6:G6"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="F3:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
CSS Flexbox & Grid
</commit_message>
<xml_diff>
--- a/Daily Schedule - Detailed Study Guide Plan - Week 1.xlsx
+++ b/Daily Schedule - Detailed Study Guide Plan - Week 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/54037f66d77c46de/Desktop/Full-Stack Developer Study Plan/Week 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="76" documentId="8_{37F14603-7835-45D1-9366-2EF83A7B62AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7030D637-48BE-447E-9F36-D3C2E739E95E}"/>
+  <xr:revisionPtr revIDLastSave="89" documentId="8_{37F14603-7835-45D1-9366-2EF83A7B62AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80C130D8-ED12-4FC6-9012-95957013ECF5}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{131ED3EB-DB14-4793-ADA5-E51D81EA1C6E}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="84">
   <si>
     <t>Day 1 - Introduction to HTML - 02/27/2025</t>
   </si>
@@ -291,7 +291,7 @@
     <t>https://www.youtube.com/watch?v=FHb9JobDs2o</t>
   </si>
   <si>
-    <t>not yet done</t>
+    <t>In Progress</t>
   </si>
 </sst>
 </file>
@@ -399,7 +399,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -483,18 +483,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -513,8 +501,20 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1130,31 +1130,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
     </row>
     <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="13" t="s">
+      <c r="B2" s="8"/>
+      <c r="C2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="13" t="s">
+      <c r="D2" s="10"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="10"/>
       <c r="H2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1166,15 +1166,15 @@
       <c r="B3" s="3">
         <v>6.25E-2</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="9" t="s">
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="9"/>
+      <c r="G3" s="14"/>
       <c r="H3" s="4" t="s">
         <v>7</v>
       </c>
@@ -1186,15 +1186,15 @@
       <c r="B4" s="3">
         <v>0.10416666666666667</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="10" t="s">
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="9"/>
+      <c r="G4" s="14"/>
       <c r="H4" s="4" t="s">
         <v>7</v>
       </c>
@@ -1206,15 +1206,15 @@
       <c r="B5" s="3">
         <v>0.14583333333333334</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="9" t="s">
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="9"/>
+      <c r="G5" s="14"/>
       <c r="H5" s="4" t="s">
         <v>7</v>
       </c>
@@ -1226,15 +1226,15 @@
       <c r="B6" s="3">
         <v>0.16666666666666666</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="9" t="s">
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="9"/>
+      <c r="G6" s="14"/>
       <c r="H6" s="4" t="s">
         <v>7</v>
       </c>
@@ -1246,15 +1246,15 @@
       <c r="B7" s="3">
         <v>0.20833333333333334</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="9" t="s">
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="9"/>
+      <c r="G7" s="14"/>
       <c r="H7" s="4" t="s">
         <v>7</v>
       </c>
@@ -1266,26 +1266,21 @@
       <c r="B8" s="3">
         <v>0.25</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="9" t="s">
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="9"/>
+      <c r="G8" s="14"/>
       <c r="H8" s="4" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="C3:E3"/>
     <mergeCell ref="C5:E5"/>
     <mergeCell ref="C6:E6"/>
     <mergeCell ref="C7:E7"/>
@@ -1297,6 +1292,11 @@
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="C4:E4"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="C3:E3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F4" r:id="rId1" xr:uid="{0649C151-4FF5-41ED-8C94-466E40481E6E}"/>
@@ -1310,7 +1310,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1328,31 +1328,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
     </row>
     <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="13" t="s">
+      <c r="B2" s="8"/>
+      <c r="C2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="13" t="s">
+      <c r="D2" s="10"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="10"/>
       <c r="H2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1364,15 +1364,15 @@
       <c r="B3" s="3">
         <v>6.25E-2</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="9" t="s">
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="9"/>
+      <c r="G3" s="14"/>
       <c r="H3" s="4" t="s">
         <v>7</v>
       </c>
@@ -1386,15 +1386,15 @@
       <c r="B4" s="3">
         <v>0.10416666666666667</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="17" t="s">
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="9"/>
+      <c r="G4" s="14"/>
       <c r="H4" s="4" t="s">
         <v>7</v>
       </c>
@@ -1407,15 +1407,15 @@
       <c r="B5" s="3">
         <v>0.14583333333333334</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="9" t="s">
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="9"/>
+      <c r="G5" s="14"/>
       <c r="H5" s="4" t="s">
         <v>7</v>
       </c>
@@ -1427,15 +1427,15 @@
       <c r="B6" s="3">
         <v>0.16666666666666666</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="9" t="s">
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="9"/>
+      <c r="G6" s="14"/>
       <c r="H6" s="4" t="s">
         <v>7</v>
       </c>
@@ -1447,16 +1447,16 @@
       <c r="B7" s="3">
         <v>0.20833333333333334</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="17" t="s">
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="G7" s="9"/>
-      <c r="H7" s="7" t="s">
+      <c r="G7" s="14"/>
+      <c r="H7" s="17" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1467,27 +1467,21 @@
       <c r="B8" s="3">
         <v>0.25</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="9" t="s">
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="9"/>
+      <c r="G8" s="14"/>
       <c r="H8" s="4" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="F3:G3"/>
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="C8:E8"/>
@@ -1498,6 +1492,12 @@
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="C6:E6"/>
     <mergeCell ref="F6:G6"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="F3:G3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F4" r:id="rId1" xr:uid="{CA69D407-ADBF-4FF3-B1FE-5BA0923AB350}"/>
@@ -1513,7 +1513,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1528,31 +1528,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
     </row>
     <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="13" t="s">
+      <c r="B2" s="8"/>
+      <c r="C2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="13" t="s">
+      <c r="D2" s="10"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="10"/>
       <c r="H2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1564,15 +1564,15 @@
       <c r="B3" s="3">
         <v>6.25E-2</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="9" t="s">
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="9"/>
+      <c r="G3" s="14"/>
       <c r="H3" s="4" t="s">
         <v>7</v>
       </c>
@@ -1584,15 +1584,15 @@
       <c r="B4" s="3">
         <v>0.10416666666666667</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="17" t="s">
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="9"/>
+      <c r="G4" s="14"/>
       <c r="H4" s="4" t="s">
         <v>7</v>
       </c>
@@ -1604,16 +1604,18 @@
       <c r="B5" s="3">
         <v>0.14583333333333334</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="9" t="s">
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="1"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="17" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="6" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
@@ -1622,16 +1624,18 @@
       <c r="B6" s="3">
         <v>0.16666666666666666</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="9" t="s">
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="9"/>
-      <c r="H6" s="1"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="4" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
@@ -1640,16 +1644,18 @@
       <c r="B7" s="3">
         <v>0.20833333333333334</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="9" t="s">
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="G7" s="9"/>
-      <c r="H7" s="1"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="4" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="8" spans="1:8" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
@@ -1658,27 +1664,21 @@
       <c r="B8" s="3">
         <v>0.25</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="9" t="s">
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="G8" s="9"/>
+      <c r="G8" s="14"/>
       <c r="H8" s="4" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="F3:G3"/>
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="C8:E8"/>
@@ -1689,6 +1689,12 @@
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="C6:E6"/>
     <mergeCell ref="F6:G6"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="F3:G3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F4" r:id="rId1" xr:uid="{4257805A-436E-4161-B8F5-14DBE7520749}"/>
@@ -1703,7 +1709,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1719,31 +1725,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
     </row>
     <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="13" t="s">
+      <c r="B2" s="8"/>
+      <c r="C2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="13" t="s">
+      <c r="D2" s="10"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="10"/>
       <c r="H2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1755,16 +1761,18 @@
       <c r="B3" s="3">
         <v>6.25E-2</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="9" t="s">
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="G3" s="9"/>
-      <c r="H3" s="1"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="4" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="4" spans="1:8" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
@@ -1773,16 +1781,18 @@
       <c r="B4" s="3">
         <v>0.10416666666666667</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="17" t="s">
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="G4" s="9"/>
-      <c r="H4" s="1"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="4" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="5" spans="1:8" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
@@ -1791,16 +1801,18 @@
       <c r="B5" s="3">
         <v>0.14583333333333334</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="9" t="s">
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="1"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="4" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="6" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
@@ -1809,16 +1821,18 @@
       <c r="B6" s="3">
         <v>0.16666666666666666</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="9" t="s">
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="9"/>
-      <c r="H6" s="1"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="4" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
@@ -1827,16 +1841,18 @@
       <c r="B7" s="3">
         <v>0.20833333333333334</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="17" t="s">
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="G7" s="9"/>
-      <c r="H7" s="1"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="4" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="8" spans="1:8" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
@@ -1845,25 +1861,21 @@
       <c r="B8" s="3">
         <v>0.25</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="9" t="s">
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="G8" s="9"/>
-      <c r="H8" s="1"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="4" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="F3:G3"/>
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="C8:E8"/>
@@ -1874,6 +1886,12 @@
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="C6:E6"/>
     <mergeCell ref="F6:G6"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="F3:G3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F4" r:id="rId1" xr:uid="{DC0E6990-69A5-43AE-B703-81524696C1B6}"/>
@@ -1904,31 +1922,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
     </row>
     <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="13" t="s">
+      <c r="B2" s="8"/>
+      <c r="C2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="13" t="s">
+      <c r="D2" s="10"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="10"/>
       <c r="H2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1940,15 +1958,15 @@
       <c r="B3" s="3">
         <v>6.25E-2</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="9" t="s">
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="9"/>
+      <c r="G3" s="14"/>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1958,15 +1976,15 @@
       <c r="B4" s="3">
         <v>0.10416666666666667</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="17" t="s">
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="G4" s="9"/>
+      <c r="G4" s="14"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1976,15 +1994,15 @@
       <c r="B5" s="3">
         <v>0.14583333333333334</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="9" t="s">
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="9"/>
+      <c r="G5" s="14"/>
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -1994,15 +2012,15 @@
       <c r="B6" s="3">
         <v>0.16666666666666666</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="9" t="s">
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="9"/>
+      <c r="G6" s="14"/>
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2012,15 +2030,15 @@
       <c r="B7" s="3">
         <v>0.20833333333333334</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="9" t="s">
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="G7" s="9"/>
+      <c r="G7" s="14"/>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2030,25 +2048,19 @@
       <c r="B8" s="3">
         <v>0.25</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="9" t="s">
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="G8" s="9"/>
+      <c r="G8" s="14"/>
       <c r="H8" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="F3:G3"/>
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="C8:E8"/>
@@ -2059,6 +2071,12 @@
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="C6:E6"/>
     <mergeCell ref="F6:G6"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="F3:G3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F4" r:id="rId1" xr:uid="{7363BFB9-59B9-41E4-94A2-43DBF92C838E}"/>
@@ -2088,31 +2106,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
     </row>
     <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="13" t="s">
+      <c r="B2" s="8"/>
+      <c r="C2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="13" t="s">
+      <c r="D2" s="10"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="10"/>
       <c r="H2" s="2" t="s">
         <v>4</v>
       </c>
@@ -2124,15 +2142,15 @@
       <c r="B3" s="3">
         <v>6.25E-2</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="9" t="s">
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="G3" s="9"/>
+      <c r="G3" s="14"/>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2142,15 +2160,15 @@
       <c r="B4" s="3">
         <v>0.10416666666666667</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="17" t="s">
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="G4" s="9"/>
+      <c r="G4" s="14"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2160,15 +2178,15 @@
       <c r="B5" s="3">
         <v>0.14583333333333334</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="9" t="s">
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="G5" s="9"/>
+      <c r="G5" s="14"/>
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -2178,15 +2196,15 @@
       <c r="B6" s="3">
         <v>0.16666666666666666</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="9" t="s">
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="9"/>
+      <c r="G6" s="14"/>
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2196,15 +2214,15 @@
       <c r="B7" s="3">
         <v>0.20833333333333334</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="9" t="s">
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="G7" s="9"/>
+      <c r="G7" s="14"/>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2214,25 +2232,19 @@
       <c r="B8" s="3">
         <v>0.25</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="9" t="s">
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="G8" s="9"/>
+      <c r="G8" s="14"/>
       <c r="H8" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="F3:G3"/>
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="C8:E8"/>
@@ -2243,6 +2255,12 @@
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="C6:E6"/>
     <mergeCell ref="F6:G6"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="F3:G3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F4" r:id="rId1" xr:uid="{FC9BA8A3-E4A7-4AA4-A429-F1F08DE2C02D}"/>
@@ -2272,31 +2290,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
     </row>
     <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="13" t="s">
+      <c r="B2" s="8"/>
+      <c r="C2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="13" t="s">
+      <c r="D2" s="10"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="10"/>
       <c r="H2" s="2" t="s">
         <v>4</v>
       </c>
@@ -2308,15 +2326,15 @@
       <c r="B3" s="3">
         <v>6.25E-2</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="9" t="s">
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="G3" s="9"/>
+      <c r="G3" s="14"/>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2326,15 +2344,15 @@
       <c r="B4" s="3">
         <v>0.10416666666666667</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="9" t="s">
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="G4" s="9"/>
+      <c r="G4" s="14"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2344,15 +2362,15 @@
       <c r="B5" s="3">
         <v>0.14583333333333334</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="9" t="s">
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="G5" s="9"/>
+      <c r="G5" s="14"/>
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -2362,15 +2380,15 @@
       <c r="B6" s="3">
         <v>0.16666666666666666</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="9" t="s">
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="9"/>
+      <c r="G6" s="14"/>
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -2380,15 +2398,15 @@
       <c r="B7" s="3">
         <v>0.20833333333333334</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="9" t="s">
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="G7" s="9"/>
+      <c r="G7" s="14"/>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -2398,25 +2416,19 @@
       <c r="B8" s="3">
         <v>0.25</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="9" t="s">
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="G8" s="9"/>
+      <c r="G8" s="14"/>
       <c r="H8" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="F3:G3"/>
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="C8:E8"/>
@@ -2427,6 +2439,12 @@
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="C6:E6"/>
     <mergeCell ref="F6:G6"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="F3:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>